<commit_message>
Update performance dashboard 2025-12-22 23:03
</commit_message>
<xml_diff>
--- a/performance-dashboard/archive/Trading_Performance_20251222.xlsx
+++ b/performance-dashboard/archive/Trading_Performance_20251222.xlsx
@@ -546,11 +546,11 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+411.13%</t>
+          <t>+404.56%</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>23.326</v>
+        <v>22.95</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -573,7 +573,7 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -619,11 +619,11 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+373.65%</t>
+          <t>+367.84%</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>22.697</v>
+        <v>22.318</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -646,7 +646,7 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -692,11 +692,11 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+153.60%</t>
+          <t>+151.73%</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>26.173</v>
+        <v>25.511</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -719,7 +719,7 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -765,11 +765,11 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+41.30%</t>
+          <t>+40.91%</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>13.049</v>
+        <v>12.248</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -838,11 +838,11 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+4.22%</t>
+          <t>+4.18%</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>11.915</v>
+        <v>6.135</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -865,7 +865,7 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -911,11 +911,11 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>+24.45%</t>
+          <t>+24.23%</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>13.689</v>
+        <v>12.391</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -938,7 +938,7 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -984,11 +984,11 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>+68.26%</t>
+          <t>+67.56%</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>15.111</v>
+        <v>14.475</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -1011,7 +1011,7 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -1057,11 +1057,11 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>+20.10%</t>
+          <t>+19.93%</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>25.578</v>
+        <v>22.701</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -1084,7 +1084,7 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1130,11 +1130,11 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>+7.41%</t>
+          <t>+7.35%</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>18.345</v>
+        <v>13.169</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1203,11 +1203,11 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>+2.73%</t>
+          <t>+2.71%</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>11.068</v>
+        <v>2.863</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -1230,7 +1230,7 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1276,11 +1276,11 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>+15.75%</t>
+          <t>+15.62%</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>11.225</v>
+        <v>9.656000000000001</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1303,7 +1303,7 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1349,11 +1349,11 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>+185.16%</t>
+          <t>+182.80%</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>18.431</v>
+        <v>18.009</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1376,7 +1376,7 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
@@ -1422,11 +1422,11 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>+270.57%</t>
+          <t>+266.74%</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>17.454</v>
+        <v>17.121</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1449,7 +1449,7 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
@@ -1495,11 +1495,11 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>+6.04%</t>
+          <t>+5.99%</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>17.782</v>
+        <v>11.68</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1522,7 +1522,7 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N15" t="inlineStr">
         <is>
@@ -1568,11 +1568,11 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>+51.62%</t>
+          <t>+51.12%</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>12.851</v>
+        <v>12.187</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1595,7 +1595,7 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N16" t="inlineStr">
         <is>
@@ -1737,11 +1737,11 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+411.13%</t>
+          <t>+404.56%</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>23.326</v>
+        <v>22.95</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -1764,7 +1764,7 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -1810,11 +1810,11 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+373.65%</t>
+          <t>+367.84%</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>22.697</v>
+        <v>22.318</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -1837,7 +1837,7 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -1883,11 +1883,11 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+153.60%</t>
+          <t>+151.73%</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>26.173</v>
+        <v>25.511</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -1910,7 +1910,7 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -1956,11 +1956,11 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+41.30%</t>
+          <t>+40.91%</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>13.049</v>
+        <v>12.248</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -1983,7 +1983,7 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -2029,11 +2029,11 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+4.22%</t>
+          <t>+4.18%</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>11.915</v>
+        <v>6.135</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -2056,7 +2056,7 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -2198,11 +2198,11 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+24.45%</t>
+          <t>+24.23%</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>13.689</v>
+        <v>12.391</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -2225,7 +2225,7 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -2271,11 +2271,11 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+68.26%</t>
+          <t>+67.56%</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>15.111</v>
+        <v>14.475</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -2298,7 +2298,7 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -2344,11 +2344,11 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+20.10%</t>
+          <t>+19.93%</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>25.578</v>
+        <v>22.701</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -2371,7 +2371,7 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -2417,11 +2417,11 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+7.41%</t>
+          <t>+7.35%</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>18.345</v>
+        <v>13.169</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -2444,7 +2444,7 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -2490,11 +2490,11 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+2.73%</t>
+          <t>+2.71%</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>11.068</v>
+        <v>2.863</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -2517,7 +2517,7 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -2659,11 +2659,11 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+15.75%</t>
+          <t>+15.62%</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>11.225</v>
+        <v>9.656000000000001</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -2686,7 +2686,7 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -2732,11 +2732,11 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+185.16%</t>
+          <t>+182.80%</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>18.431</v>
+        <v>18.009</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -2759,7 +2759,7 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -2805,11 +2805,11 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+270.57%</t>
+          <t>+266.74%</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>17.454</v>
+        <v>17.121</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -2832,7 +2832,7 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -2878,11 +2878,11 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+6.04%</t>
+          <t>+5.99%</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>17.782</v>
+        <v>11.68</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -2905,7 +2905,7 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -2951,11 +2951,11 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+51.62%</t>
+          <t>+51.12%</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>12.851</v>
+        <v>12.187</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -2978,7 +2978,7 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update performance dashboard 2025-12-22 23:33
</commit_message>
<xml_diff>
--- a/performance-dashboard/archive/Trading_Performance_20251222.xlsx
+++ b/performance-dashboard/archive/Trading_Performance_20251222.xlsx
@@ -546,7 +546,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+404.56%</t>
+          <t>+236.65%</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -573,7 +573,7 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -619,7 +619,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+367.84%</t>
+          <t>+218.11%</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -646,7 +646,7 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -692,7 +692,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+151.73%</t>
+          <t>+99.85%</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -719,7 +719,7 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -765,7 +765,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+40.91%</t>
+          <t>+29.33%</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -838,7 +838,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+4.18%</t>
+          <t>+3.12%</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -865,7 +865,7 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -911,7 +911,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>+24.23%</t>
+          <t>+17.67%</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -938,7 +938,7 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -984,7 +984,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>+67.56%</t>
+          <t>+29.45%</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -1011,7 +1011,7 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>+19.93%</t>
+          <t>+14.60%</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -1084,7 +1084,7 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>+7.35%</t>
+          <t>+5.46%</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>+2.71%</t>
+          <t>+2.03%</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -1230,7 +1230,7 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>+15.62%</t>
+          <t>+11.50%</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -1303,7 +1303,7 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>+182.80%</t>
+          <t>+118.08%</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -1376,7 +1376,7 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
@@ -1422,7 +1422,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>+266.74%</t>
+          <t>+165.01%</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1449,7 +1449,7 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>+5.99%</t>
+          <t>+4.46%</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1522,7 +1522,7 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N15" t="inlineStr">
         <is>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>+51.12%</t>
+          <t>+36.30%</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1595,7 +1595,7 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N16" t="inlineStr">
         <is>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+404.56%</t>
+          <t>+236.65%</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -1764,7 +1764,7 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+367.84%</t>
+          <t>+218.11%</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -1837,7 +1837,7 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+151.73%</t>
+          <t>+99.85%</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -1910,7 +1910,7 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+40.91%</t>
+          <t>+29.33%</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -1983,7 +1983,7 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -2029,7 +2029,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+4.18%</t>
+          <t>+3.12%</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -2056,7 +2056,7 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+24.23%</t>
+          <t>+17.67%</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -2225,7 +2225,7 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -2271,7 +2271,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+67.56%</t>
+          <t>+29.45%</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -2298,7 +2298,7 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -2344,7 +2344,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+19.93%</t>
+          <t>+14.60%</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -2371,7 +2371,7 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -2417,7 +2417,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+7.35%</t>
+          <t>+5.46%</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -2444,7 +2444,7 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -2490,7 +2490,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+2.71%</t>
+          <t>+2.03%</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -2517,7 +2517,7 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -2659,7 +2659,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+15.62%</t>
+          <t>+11.50%</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -2686,7 +2686,7 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -2732,7 +2732,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+182.80%</t>
+          <t>+118.08%</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -2759,7 +2759,7 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -2805,7 +2805,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+266.74%</t>
+          <t>+165.01%</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -2832,7 +2832,7 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -2878,7 +2878,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+5.99%</t>
+          <t>+4.46%</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -2905,7 +2905,7 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -2951,7 +2951,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+51.12%</t>
+          <t>+36.30%</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -2978,7 +2978,7 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>

</xml_diff>